<commit_message>
updated genotype list with available data
</commit_message>
<xml_diff>
--- a/data/conetta_data_5geno.xlsx
+++ b/data/conetta_data_5geno.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hputnam/MyProjects/Apulchra_Plasticity/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{33DA1047-E7A7-414D-A83C-D0BE03F37C1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF44A860-E160-4C4D-BF86-5365C3D34A25}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36600" yWindow="2560" windowWidth="34420" windowHeight="18280"/>
+    <workbookView xWindow="-37780" yWindow="3400" windowWidth="37560" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="conetta_data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="70">
   <si>
     <t>colony_id</t>
   </si>
@@ -150,9 +150,6 @@
     <t>ACR-150</t>
   </si>
   <si>
-    <t>ACR-173</t>
-  </si>
-  <si>
     <t>ACR-178</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>ACR-187</t>
   </si>
   <si>
-    <t>ACR-193</t>
-  </si>
-  <si>
     <t>ACR-225</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Mahana Low</t>
   </si>
   <si>
-    <t>ACR-228</t>
-  </si>
-  <si>
     <t>ACR-234</t>
   </si>
   <si>
@@ -207,18 +198,12 @@
     <t>ACR-350</t>
   </si>
   <si>
-    <t>ACR-363</t>
-  </si>
-  <si>
     <t>ACR-368</t>
   </si>
   <si>
     <t>ACR-374</t>
   </si>
   <si>
-    <t>ACR-379</t>
-  </si>
-  <si>
     <t>ACR-389</t>
   </si>
   <si>
@@ -234,19 +219,31 @@
     <t>Genotype15</t>
   </si>
   <si>
-    <t>Genotype7</t>
-  </si>
-  <si>
     <t>Genotype6</t>
   </si>
   <si>
     <t>Genotype4</t>
+  </si>
+  <si>
+    <t>colony_id_corr</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>Hilton</t>
+  </si>
+  <si>
+    <t>Acropora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -389,7 +386,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +572,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -736,7 +739,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -745,10 +748,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1103,11 +1103,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34:W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1227,7 +1227,7 @@
         <v>39</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
@@ -1331,10 +1331,10 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -1343,10 +1343,10 @@
         <v>43831</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H3">
         <v>8.3438633121383804E-2</v>
@@ -1438,10 +1438,10 @@
         <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -1450,10 +1450,10 @@
         <v>43831</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>5.7637784168016001E-2</v>
@@ -1548,7 +1548,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>38</v>
@@ -1652,10 +1652,10 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -1664,10 +1664,10 @@
         <v>44136</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="7" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C7" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>38</v>
@@ -1765,7 +1765,7 @@
         <v>44136</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
@@ -1775,10 +1775,10 @@
         <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -1882,10 +1882,10 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
@@ -1894,10 +1894,10 @@
         <v>43831</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H9">
         <v>0.37964123940332301</v>
@@ -1989,10 +1989,10 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -2001,10 +2001,10 @@
         <v>43831</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H10">
         <v>0.14399719983761</v>
@@ -2096,10 +2096,10 @@
         <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -2108,10 +2108,10 @@
         <v>43831</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H11">
         <v>0.109845286826594</v>
@@ -2203,10 +2203,10 @@
         <v>96</v>
       </c>
       <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -2215,10 +2215,10 @@
         <v>43831</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H12">
         <v>0.104563473529672</v>
@@ -2310,10 +2310,10 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
         <v>38</v>
@@ -2417,10 +2417,10 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
         <v>38</v>
@@ -2429,10 +2429,10 @@
         <v>44136</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H14">
         <v>0.703251588061649</v>
@@ -2524,10 +2524,10 @@
         <v>97</v>
       </c>
       <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="D15" t="s">
         <v>38</v>
@@ -2536,10 +2536,10 @@
         <v>44136</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
         <v>37</v>
@@ -2631,10 +2631,10 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
@@ -2738,10 +2738,10 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
@@ -2845,10 +2845,10 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
         <v>34</v>
@@ -2857,10 +2857,10 @@
         <v>43831</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H18">
         <v>0.107163132737008</v>
@@ -2952,10 +2952,10 @@
         <v>92</v>
       </c>
       <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -2964,10 +2964,10 @@
         <v>43831</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H19">
         <v>9.4957809357454806E-2</v>
@@ -3059,10 +3059,10 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
         <v>38</v>
@@ -3166,10 +3166,10 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>38</v>
@@ -3178,10 +3178,10 @@
         <v>44136</v>
       </c>
       <c r="F21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H21" t="s">
         <v>37</v>
@@ -3273,10 +3273,10 @@
         <v>93</v>
       </c>
       <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D22" t="s">
         <v>38</v>
@@ -3285,10 +3285,10 @@
         <v>44136</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H22" t="s">
         <v>37</v>
@@ -3375,122 +3375,122 @@
         <v>1.4024847605224901E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8">
-        <v>10</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="8" t="s">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="1">
         <v>43831</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="8">
-        <v>0.12499655706148</v>
-      </c>
-      <c r="I23" s="8">
-        <v>1.2823275970710999</v>
-      </c>
-      <c r="J23" s="8">
-        <v>0.94866072232299603</v>
-      </c>
-      <c r="K23" s="8">
-        <v>310.29710854025501</v>
-      </c>
-      <c r="L23" s="8">
-        <v>376.09490774303299</v>
-      </c>
-      <c r="M23" s="8">
-        <v>1.7946828969784601</v>
-      </c>
-      <c r="N23" s="8">
-        <v>1.9454937818768601</v>
-      </c>
-      <c r="O23" s="8">
-        <v>476.55954531965898</v>
-      </c>
-      <c r="P23" s="8">
-        <v>22.9270586292849</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>800364.333546101</v>
-      </c>
-      <c r="R23" s="8">
-        <v>0.74747255757372</v>
-      </c>
-      <c r="S23" s="8">
-        <v>1.8183452792541999E-3</v>
-      </c>
-      <c r="T23" s="8">
-        <v>0.44581205394815299</v>
-      </c>
-      <c r="U23" s="8">
-        <v>10.9261086358892</v>
-      </c>
-      <c r="V23" s="8">
-        <v>29.399999999999</v>
-      </c>
-      <c r="W23" s="8">
-        <v>18350000</v>
-      </c>
-      <c r="X23" s="8">
-        <v>1679463.4404169701</v>
-      </c>
-      <c r="Y23" s="8">
-        <v>624149.65986396605</v>
-      </c>
-      <c r="Z23" s="8">
-        <v>3.76591532916343</v>
-      </c>
-      <c r="AA23" s="8">
-        <v>1.39955102040821</v>
-      </c>
-      <c r="AB23" s="8">
-        <v>4.0823729185235296</v>
-      </c>
-      <c r="AC23" s="8">
-        <v>1.5171581632653599</v>
-      </c>
-      <c r="AD23" s="8">
-        <v>0.47655954531965899</v>
-      </c>
-      <c r="AE23" s="8">
-        <v>0.37163634815950802</v>
-      </c>
-      <c r="AF23" s="8">
-        <v>4.6453263998839998E-2</v>
-      </c>
-      <c r="AG23" s="8">
-        <v>5.9568302399741799E-2</v>
-      </c>
-      <c r="AH23" s="11">
-        <v>2.24233242506812E-6</v>
-      </c>
-      <c r="AI23" s="11">
-        <v>2.4307602179836501E-6</v>
+      <c r="H23">
+        <v>0.16359918567252099</v>
+      </c>
+      <c r="I23">
+        <v>0.85124911043927698</v>
+      </c>
+      <c r="J23">
+        <v>0.81850876003773398</v>
+      </c>
+      <c r="K23">
+        <v>193.904725252943</v>
+      </c>
+      <c r="L23">
+        <v>238.20651188998701</v>
+      </c>
+      <c r="M23">
+        <v>0.81157803711213305</v>
+      </c>
+      <c r="N23">
+        <v>0.52900630415619998</v>
+      </c>
+      <c r="O23">
+        <v>391.15904761594498</v>
+      </c>
+      <c r="P23">
+        <v>24.434680453606301</v>
+      </c>
+      <c r="Q23">
+        <v>403797.65495195799</v>
+      </c>
+      <c r="R23">
+        <v>0.73954322658687699</v>
+      </c>
+      <c r="S23">
+        <v>2.6780705273302301E-3</v>
+      </c>
+      <c r="T23">
+        <v>0.41539997198849898</v>
+      </c>
+      <c r="U23">
+        <v>9.5578463350326093</v>
+      </c>
+      <c r="V23">
+        <v>20.800000000000399</v>
+      </c>
+      <c r="W23">
+        <v>9866666.6666666698</v>
+      </c>
+      <c r="X23">
+        <v>1032310.66087578</v>
+      </c>
+      <c r="Y23">
+        <v>474358.97435896599</v>
+      </c>
+      <c r="Z23">
+        <v>2.07480318315165</v>
+      </c>
+      <c r="AA23">
+        <v>0.95339663461536805</v>
+      </c>
+      <c r="AB23">
+        <v>1.35240717907565</v>
+      </c>
+      <c r="AC23">
+        <v>0.62144711538460495</v>
+      </c>
+      <c r="AD23">
+        <v>0.391159047615945</v>
+      </c>
+      <c r="AE23">
+        <v>0.45951184303040599</v>
+      </c>
+      <c r="AF23">
+        <v>7.5175763326653697E-2</v>
+      </c>
+      <c r="AG23">
+        <v>6.3993301658407595E-2</v>
+      </c>
+      <c r="AH23" s="2">
+        <v>2.0098631756756798E-6</v>
+      </c>
+      <c r="AI23" s="2">
+        <v>1.3100777027027E-6</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
         <v>34</v>
@@ -3505,99 +3505,99 @@
         <v>36</v>
       </c>
       <c r="H24">
-        <v>0.107085858043991</v>
+        <v>0.118145705056098</v>
       </c>
       <c r="I24">
-        <v>1.1007324043702</v>
+        <v>1.62711338153373</v>
       </c>
       <c r="J24">
-        <v>0.88768742287924296</v>
+        <v>1.1796572016118601</v>
       </c>
       <c r="K24">
-        <v>210.20438173779701</v>
+        <v>390.73500744149101</v>
       </c>
       <c r="L24">
-        <v>255.43205593349199</v>
+        <v>463.48324672986001</v>
       </c>
       <c r="M24">
-        <v>2.2778059271080502</v>
+        <v>2.0295595375387299</v>
       </c>
       <c r="N24">
-        <v>2.4747837662449501</v>
+        <v>1.7943806371553099</v>
       </c>
       <c r="O24">
-        <v>393.49230150207597</v>
+        <v>474.27945999201802</v>
       </c>
       <c r="P24">
-        <v>27.036543924612701</v>
+        <v>15.364633026640099</v>
       </c>
       <c r="Q24">
-        <v>543955.12635320495</v>
+        <v>698302.82624152605</v>
       </c>
       <c r="R24">
-        <v>1.1637588104748999</v>
+        <v>0.99959557245467501</v>
       </c>
       <c r="S24">
-        <v>2.5850709365505499E-3</v>
+        <v>2.7294530307438599E-3</v>
       </c>
       <c r="T24">
-        <v>0.48022624827617699</v>
+        <v>0.434660122006084</v>
       </c>
       <c r="U24">
-        <v>10.638671893557801</v>
+        <v>7.2871298548504004</v>
       </c>
       <c r="V24">
-        <v>29.7599999999996</v>
+        <v>25.000000000001201</v>
       </c>
       <c r="W24">
-        <v>14706666.6666667</v>
+        <v>10729166.6666667</v>
       </c>
       <c r="X24">
-        <v>1382378.0650263501</v>
+        <v>1472344.65151259</v>
       </c>
       <c r="Y24">
-        <v>494175.62724015099</v>
+        <v>429166.66666664602</v>
       </c>
       <c r="Z24">
-        <v>5.7886924811819496</v>
+        <v>4.2792482254510604</v>
       </c>
       <c r="AA24">
-        <v>2.0693548387097098</v>
+        <v>1.24733749999994</v>
       </c>
       <c r="AB24">
-        <v>6.2892812814837002</v>
+        <v>3.7833825592732002</v>
       </c>
       <c r="AC24">
-        <v>2.2483064516129398</v>
+        <v>1.10279999999995</v>
       </c>
       <c r="AD24">
-        <v>0.39349230150207598</v>
+        <v>0.47427945999201798</v>
       </c>
       <c r="AE24">
-        <v>0.35748225448783599</v>
+        <v>0.29148519419400098</v>
       </c>
       <c r="AF24">
-        <v>3.8281293957330403E-2</v>
+        <v>3.4437723781464001E-2</v>
       </c>
       <c r="AG24">
-        <v>4.2137460740054901E-2</v>
+        <v>5.6034081194382399E-2</v>
       </c>
       <c r="AH24" s="2">
-        <v>4.18748866727108E-6</v>
+        <v>2.9064174757281601E-6</v>
       </c>
       <c r="AI24" s="2">
-        <v>4.54961015412511E-6</v>
+        <v>2.5696310679611601E-6</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
@@ -3606,105 +3606,105 @@
         <v>43831</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H25">
-        <v>5.7067015500173499E-2</v>
+        <v>0.14520803234691501</v>
       </c>
       <c r="I25">
-        <v>0.58302676810416998</v>
+        <v>1.39281593917236</v>
       </c>
       <c r="J25">
-        <v>0.72878346013020301</v>
+        <v>1.3207737354219999</v>
       </c>
       <c r="K25">
-        <v>322.60814501763798</v>
+        <v>567.98073436729896</v>
       </c>
       <c r="L25">
-        <v>402.80902960625201</v>
+        <v>685.60163902360796</v>
       </c>
       <c r="M25">
-        <v>1.6197200833402401</v>
+        <v>2.7960579861651298</v>
       </c>
       <c r="N25">
-        <v>2.6518417283629301</v>
+        <v>3.6854390031857398</v>
       </c>
       <c r="O25">
-        <v>286.91464925072</v>
+        <v>617.14146519447399</v>
       </c>
       <c r="P25">
-        <v>23.052114817477399</v>
+        <v>13.325522402500299</v>
       </c>
       <c r="Q25">
-        <v>311674.74054548098</v>
+        <v>906245.18209692102</v>
       </c>
       <c r="R25">
-        <v>0.67876792415929299</v>
+        <v>1.1238176537978899</v>
       </c>
       <c r="S25">
-        <v>2.2999569273491698E-3</v>
+        <v>3.3335935485625302E-3</v>
       </c>
       <c r="T25">
-        <v>0.386541232581671</v>
+        <v>0.60752824656641302</v>
       </c>
       <c r="U25">
-        <v>6.6139894373438697</v>
+        <v>8.2237324199608093</v>
       </c>
       <c r="V25">
-        <v>13.440000000000101</v>
+        <v>18.560000000000802</v>
       </c>
       <c r="W25">
-        <v>7184761.9047619198</v>
+        <v>12076190.4761905</v>
       </c>
       <c r="X25">
-        <v>1086297.7591399499</v>
+        <v>1468456.1534223701</v>
       </c>
       <c r="Y25">
-        <v>534580.49886620895</v>
+        <v>650656.814449889</v>
       </c>
       <c r="Z25">
-        <v>5.6453028368197797</v>
+        <v>4.5306597333952201</v>
       </c>
       <c r="AA25">
-        <v>2.7781230158730001</v>
+        <v>2.0074856321838199</v>
       </c>
       <c r="AB25">
-        <v>9.2426153048937607</v>
+        <v>5.9717896317732997</v>
       </c>
       <c r="AC25">
-        <v>4.5484047619047301</v>
+        <v>2.6460344827585001</v>
       </c>
       <c r="AD25">
-        <v>0.28691464925072002</v>
+        <v>0.61714146519447399</v>
       </c>
       <c r="AE25">
-        <v>0.492112309326176</v>
+        <v>0.44308903124786903</v>
       </c>
       <c r="AF25">
-        <v>2.8083380784143099E-2</v>
+        <v>6.4340086382003794E-2</v>
       </c>
       <c r="AG25">
-        <v>1.6373362736017701E-2</v>
+        <v>8.9613897840581505E-2</v>
       </c>
       <c r="AH25" s="2">
-        <v>5.1968282078473001E-6</v>
+        <v>3.0853217665615099E-6</v>
       </c>
       <c r="AI25" s="2">
-        <v>8.5083626723223806E-6</v>
+        <v>4.0667129337539404E-6</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
@@ -3713,1492 +3713,856 @@
         <v>43831</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H26">
-        <v>9.6672020970682795E-2</v>
+        <v>0.17300857271987699</v>
       </c>
       <c r="I26">
-        <v>0.92233156938580896</v>
+        <v>1.3006157314800499</v>
       </c>
       <c r="J26">
-        <v>0.68854613686785704</v>
+        <v>1.22521771806093</v>
       </c>
       <c r="K26">
-        <v>153.299192928331</v>
+        <v>226.42023429765501</v>
       </c>
       <c r="L26">
-        <v>185.01074570631101</v>
+        <v>273.93040750338503</v>
       </c>
       <c r="M26">
-        <v>1.22032633107178</v>
+        <v>1.9605431270987701</v>
       </c>
       <c r="N26">
-        <v>0.40031111635446498</v>
+        <v>1.79311555513381</v>
       </c>
       <c r="O26">
-        <v>359.85304720165601</v>
+        <v>554.03399555536805</v>
       </c>
       <c r="P26">
-        <v>39.0315166420827</v>
+        <v>26.525897822826401</v>
       </c>
       <c r="Q26">
-        <v>676447.65177561797</v>
+        <v>1016825.9865274701</v>
       </c>
       <c r="R26">
-        <v>0.83104168000341305</v>
+        <v>1.4219122130617301</v>
       </c>
       <c r="S26">
-        <v>2.6843974259765798E-3</v>
+        <v>3.0960478508432199E-3</v>
       </c>
       <c r="T26">
-        <v>0.3611534525988</v>
+        <v>0.64925132544984798</v>
       </c>
       <c r="U26">
-        <v>14.0456102005556</v>
+        <v>14.696249156474</v>
       </c>
       <c r="V26">
-        <v>36.000000000000497</v>
+        <v>34.500000000000398</v>
       </c>
       <c r="W26">
-        <v>26402777.777777798</v>
+        <v>26972222.222222202</v>
       </c>
       <c r="X26">
-        <v>1879788.5888028799</v>
+        <v>1835313.3466262999</v>
       </c>
       <c r="Y26">
-        <v>733410.49382715102</v>
+        <v>781803.54267309804</v>
       </c>
       <c r="Z26">
-        <v>3.3911796511422398</v>
+        <v>3.5386693647445</v>
       </c>
       <c r="AA26">
-        <v>1.32308854166665</v>
+        <v>1.5073961352656799</v>
       </c>
       <c r="AB26">
-        <v>1.1124294193627799</v>
+        <v>3.2364720748523301</v>
       </c>
       <c r="AC26">
-        <v>0.43402083333332803</v>
+        <v>1.3786666666666501</v>
       </c>
       <c r="AD26">
-        <v>0.35985304720165601</v>
+        <v>0.55403399555536803</v>
       </c>
       <c r="AE26">
-        <v>0.39015583890431699</v>
+        <v>0.42597823641952998</v>
       </c>
       <c r="AF26">
-        <v>3.7717153440392497E-2</v>
+        <v>7.3697886692673104E-2</v>
       </c>
       <c r="AG26">
-        <v>3.4787721325442597E-2</v>
+        <v>9.5852630809324796E-2</v>
       </c>
       <c r="AH26" s="2">
-        <v>1.80402183061547E-6</v>
+        <v>1.9281009268795099E-6</v>
       </c>
       <c r="AI26" s="2">
-        <v>5.9178432403997899E-7</v>
+        <v>1.7634438722966001E-6</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27">
+        <v>0.115848259320189</v>
+      </c>
+      <c r="I27">
+        <v>1.1061535598938801</v>
+      </c>
+      <c r="J27">
+        <v>0.91055323527847798</v>
+      </c>
+      <c r="K27">
+        <v>320.19098655660099</v>
+      </c>
+      <c r="L27">
+        <v>389.81795728089702</v>
+      </c>
+      <c r="M27">
+        <v>0.89823378724712399</v>
+      </c>
+      <c r="N27">
+        <v>0.35851516050365601</v>
+      </c>
+      <c r="O27">
+        <v>423.348706063836</v>
+      </c>
+      <c r="P27">
+        <v>29.652302527640501</v>
+      </c>
+      <c r="Q27">
+        <v>826242.75053049403</v>
+      </c>
+      <c r="R27">
+        <v>0.91965399481760002</v>
+      </c>
+      <c r="S27">
+        <v>3.5236420866743999E-3</v>
+      </c>
+      <c r="T27">
+        <v>0.50477847293036304</v>
+      </c>
+      <c r="U27">
+        <v>12.553263906890001</v>
+      </c>
+      <c r="V27">
+        <v>32.799999999999898</v>
+      </c>
+      <c r="W27">
+        <v>24500000</v>
+      </c>
+      <c r="X27">
+        <v>1951683.65627626</v>
+      </c>
+      <c r="Y27">
+        <v>746951.21951219696</v>
+      </c>
+      <c r="Z27">
+        <v>2.1217350481559798</v>
+      </c>
+      <c r="AA27">
+        <v>0.81203353658536703</v>
+      </c>
+      <c r="AB27">
+        <v>0.84685545359762104</v>
+      </c>
+      <c r="AC27">
+        <v>0.32410975609756199</v>
+      </c>
+      <c r="AD27">
+        <v>0.42334870606383601</v>
+      </c>
+      <c r="AE27">
+        <v>0.38272146057591599</v>
+      </c>
+      <c r="AF27">
+        <v>4.4337615012200203E-2</v>
+      </c>
+      <c r="AG27">
+        <v>4.9044210682949702E-2</v>
+      </c>
+      <c r="AH27" s="2">
+        <v>1.0871306122448999E-6</v>
+      </c>
+      <c r="AI27" s="2">
+        <v>4.3391020408163301E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28">
+        <v>0.106621041740164</v>
+      </c>
+      <c r="I28">
+        <v>0.80795751460282095</v>
+      </c>
+      <c r="J28">
+        <v>0.67910222132567</v>
+      </c>
+      <c r="K28">
+        <v>165.04621781058901</v>
+      </c>
+      <c r="L28">
+        <v>200.24809090371599</v>
+      </c>
+      <c r="M28">
+        <v>0.85117801777082602</v>
+      </c>
+      <c r="N28">
+        <v>0.342988412675377</v>
+      </c>
+      <c r="O28">
+        <v>415.97278121295602</v>
+      </c>
+      <c r="P28">
+        <v>28.7143811161963</v>
+      </c>
+      <c r="Q28">
+        <v>563790.27719171601</v>
+      </c>
+      <c r="R28">
+        <v>0.97246464388892795</v>
+      </c>
+      <c r="S28">
+        <v>1.85183860368685E-3</v>
+      </c>
+      <c r="T28">
+        <v>0.58614835737684901</v>
+      </c>
+      <c r="U28">
+        <v>11.9444009737129</v>
+      </c>
+      <c r="V28">
+        <v>23.200000000000099</v>
+      </c>
+      <c r="W28">
+        <v>16188888.888888899</v>
+      </c>
+      <c r="X28">
+        <v>1355353.76989747</v>
+      </c>
+      <c r="Y28">
+        <v>697796.93486589601</v>
+      </c>
+      <c r="Z28">
+        <v>2.0462348889483399</v>
+      </c>
+      <c r="AA28">
+        <v>1.0534935344827501</v>
+      </c>
+      <c r="AB28">
+        <v>0.82454532643996703</v>
+      </c>
+      <c r="AC28">
+        <v>0.42451293103448001</v>
+      </c>
+      <c r="AD28">
+        <v>0.415972781212956</v>
+      </c>
+      <c r="AE28">
+        <v>0.51484486955658904</v>
+      </c>
+      <c r="AF28">
+        <v>5.48932963267025E-2</v>
+      </c>
+      <c r="AG28">
+        <v>4.4351451268478698E-2</v>
+      </c>
+      <c r="AH28" s="2">
+        <v>1.50974227865477E-6</v>
+      </c>
+      <c r="AI28" s="2">
+        <v>6.0836170212766E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E29" s="1">
         <v>44136</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F29" t="s">
         <v>35</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G29" t="s">
         <v>36</v>
       </c>
-      <c r="H27">
-        <v>0.68033430936436301</v>
-      </c>
-      <c r="I27">
-        <v>1.0199403105239899</v>
-      </c>
-      <c r="J27">
-        <v>0.79995318472465404</v>
-      </c>
-      <c r="K27">
-        <v>237.786084159414</v>
-      </c>
-      <c r="L27">
-        <v>285.333301576488</v>
-      </c>
-      <c r="M27">
-        <v>0.81171249654014499</v>
-      </c>
-      <c r="N27">
-        <v>0.21270255211089101</v>
-      </c>
-      <c r="O27">
-        <v>326.08314373921502</v>
-      </c>
-      <c r="P27">
-        <v>35.002048288158697</v>
-      </c>
-      <c r="Q27">
-        <v>279983.614653642</v>
-      </c>
-      <c r="R27">
-        <v>0.62296384269840799</v>
-      </c>
-      <c r="S27">
-        <v>2.2933780446145299E-3</v>
-      </c>
-      <c r="T27">
-        <v>0.14851227591364299</v>
-      </c>
-      <c r="U27">
-        <v>11.4135779431146</v>
-      </c>
-      <c r="V27">
-        <v>35.700000000000301</v>
-      </c>
-      <c r="W27">
-        <v>9800000</v>
-      </c>
-      <c r="X27">
-        <v>858626.45778942399</v>
-      </c>
-      <c r="Y27">
-        <v>274509.803921566</v>
-      </c>
-      <c r="Z27">
-        <v>2.4892807620540802</v>
-      </c>
-      <c r="AA27">
-        <v>0.79584313725489697</v>
-      </c>
-      <c r="AB27">
-        <v>0.65229545345956297</v>
-      </c>
-      <c r="AC27">
-        <v>0.20854411764705699</v>
-      </c>
-      <c r="AD27">
-        <v>0.32608314373921499</v>
-      </c>
-      <c r="AE27">
-        <v>0.31970806563345999</v>
-      </c>
-      <c r="AF27">
-        <v>0.217508366030957</v>
-      </c>
-      <c r="AG27">
-        <v>0.22184555039117901</v>
-      </c>
-      <c r="AH27" s="2">
-        <v>2.89914285714286E-6</v>
-      </c>
-      <c r="AI27" s="2">
-        <v>7.5969642857142904E-7</v>
+      <c r="H29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29">
+        <v>0.50530402714327105</v>
+      </c>
+      <c r="J29">
+        <v>0.503330183287229</v>
+      </c>
+      <c r="K29">
+        <v>94.570806830031103</v>
+      </c>
+      <c r="L29">
+        <v>113.80196751931599</v>
+      </c>
+      <c r="M29">
+        <v>0.56168095535914497</v>
+      </c>
+      <c r="N29">
+        <v>0.299250519324749</v>
+      </c>
+      <c r="O29" t="s">
+        <v>37</v>
+      </c>
+      <c r="P29">
+        <v>30.3975412324295</v>
+      </c>
+      <c r="Q29">
+        <v>214820.006331087</v>
+      </c>
+      <c r="R29">
+        <v>0.81568123579018903</v>
+      </c>
+      <c r="S29">
+        <v>2.4365068649643798E-3</v>
+      </c>
+      <c r="T29">
+        <v>0.34856854250958602</v>
+      </c>
+      <c r="U29" t="s">
+        <v>37</v>
+      </c>
+      <c r="V29">
+        <v>15.3600000000003</v>
+      </c>
+      <c r="W29">
+        <v>6530000</v>
+      </c>
+      <c r="X29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y29">
+        <v>425130.20833332598</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA29">
+        <v>1.1115703124999801</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC29">
+        <v>0.59221874999999102</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH29" s="2">
+        <v>2.6146584992343101E-6</v>
+      </c>
+      <c r="AI29" s="2">
+        <v>1.3930290964778E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>42</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="4" t="s">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E30" s="1">
         <v>44136</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="T28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="W28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="X28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI28" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>79</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="6">
-        <v>44136</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="T29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="W29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="X29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI29" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>91</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="6">
-        <v>44136</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="S30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="T30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="W30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="X30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI30" s="4" t="s">
-        <v>37</v>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30">
+        <v>1.2957911441005101</v>
+      </c>
+      <c r="J30">
+        <v>0.54482127649676604</v>
+      </c>
+      <c r="K30">
+        <v>93.391201731172899</v>
+      </c>
+      <c r="L30">
+        <v>169.05656960702501</v>
+      </c>
+      <c r="M30">
+        <v>0.640397653293721</v>
+      </c>
+      <c r="N30">
+        <v>0.32713130926779799</v>
+      </c>
+      <c r="O30">
+        <v>346.68071258500601</v>
+      </c>
+      <c r="P30">
+        <v>63.667667722229297</v>
+      </c>
+      <c r="Q30">
+        <v>196086.576540971</v>
+      </c>
+      <c r="R30">
+        <v>0.44145099385251901</v>
+      </c>
+      <c r="S30">
+        <v>1.0675887644996599E-3</v>
+      </c>
+      <c r="T30">
+        <v>0.18757983587997401</v>
+      </c>
+      <c r="U30">
+        <v>22.072352414567799</v>
+      </c>
+      <c r="V30">
+        <v>82.499999999998707</v>
+      </c>
+      <c r="W30">
+        <v>12484375</v>
+      </c>
+      <c r="X30">
+        <v>565611.43848719401</v>
+      </c>
+      <c r="Y30">
+        <v>151325.75757576001</v>
+      </c>
+      <c r="Z30">
+        <v>1.84722607877038</v>
+      </c>
+      <c r="AA30">
+        <v>0.49421363636364402</v>
+      </c>
+      <c r="AB30">
+        <v>0.94360977519793698</v>
+      </c>
+      <c r="AC30">
+        <v>0.25245681818182197</v>
+      </c>
+      <c r="AD30">
+        <v>0.34668071258500599</v>
+      </c>
+      <c r="AE30">
+        <v>0.26754366563112902</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH30" s="2">
+        <v>3.2658923654568202E-6</v>
+      </c>
+      <c r="AI30" s="2">
+        <v>1.6683003754693401E-6</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="1">
+        <v>44136</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+      <c r="H31">
+        <v>0.19146997167881399</v>
+      </c>
+      <c r="I31">
+        <v>0.693497776956703</v>
+      </c>
+      <c r="J31">
+        <v>0.735195428102834</v>
+      </c>
+      <c r="K31">
+        <v>103.87543284466599</v>
+      </c>
+      <c r="L31">
+        <v>126.22317924577401</v>
+      </c>
+      <c r="M31">
+        <v>0.67091959616768004</v>
+      </c>
+      <c r="N31">
+        <v>0.26487445314631403</v>
+      </c>
+      <c r="O31">
+        <v>253.40421317115599</v>
+      </c>
+      <c r="P31">
+        <v>45.566115782910401</v>
+      </c>
+      <c r="Q31">
+        <v>196539.80598702599</v>
+      </c>
+      <c r="R31">
+        <v>0.73990593858654796</v>
+      </c>
+      <c r="S31">
+        <v>2.3155231556607602E-3</v>
+      </c>
+      <c r="T31">
+        <v>0.232428594429613</v>
+      </c>
+      <c r="U31">
+        <v>11.546645717234201</v>
+      </c>
+      <c r="V31">
+        <v>31.600000000000101</v>
+      </c>
+      <c r="W31">
+        <v>8955555.5555555597</v>
+      </c>
+      <c r="X31">
+        <v>775598.01996771595</v>
+      </c>
+      <c r="Y31">
+        <v>283403.65682137798</v>
+      </c>
+      <c r="Z31">
+        <v>2.64762605077336</v>
+      </c>
+      <c r="AA31">
+        <v>0.96744303797468101</v>
+      </c>
+      <c r="AB31">
+        <v>1.0452645985306099</v>
+      </c>
+      <c r="AC31">
+        <v>0.38193987341772001</v>
+      </c>
+      <c r="AD31">
+        <v>0.25340421317115602</v>
+      </c>
+      <c r="AE31">
+        <v>0.36540018092513199</v>
+      </c>
+      <c r="AF31">
+        <v>6.9963162293168402E-2</v>
+      </c>
+      <c r="AG31">
+        <v>4.8519297519173298E-2</v>
+      </c>
+      <c r="AH31" s="2">
+        <v>3.4136575682382101E-6</v>
+      </c>
+      <c r="AI31" s="2">
+        <v>1.3476885856079399E-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" t="s">
+        <v>14</v>
+      </c>
+      <c r="P34" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q34" t="s">
         <v>65</v>
       </c>
-      <c r="D31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="1">
-        <v>43831</v>
-      </c>
-      <c r="F31" t="s">
-        <v>35</v>
-      </c>
-      <c r="G31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31">
-        <v>0.16359918567252099</v>
-      </c>
-      <c r="I31">
-        <v>0.85124911043927698</v>
-      </c>
-      <c r="J31">
-        <v>0.81850876003773398</v>
-      </c>
-      <c r="K31">
-        <v>193.904725252943</v>
-      </c>
-      <c r="L31">
-        <v>238.20651188998701</v>
-      </c>
-      <c r="M31">
-        <v>0.81157803711213305</v>
-      </c>
-      <c r="N31">
-        <v>0.52900630415619998</v>
-      </c>
-      <c r="O31">
-        <v>391.15904761594498</v>
-      </c>
-      <c r="P31">
-        <v>24.434680453606301</v>
-      </c>
-      <c r="Q31">
-        <v>403797.65495195799</v>
-      </c>
-      <c r="R31">
-        <v>0.73954322658687699</v>
-      </c>
-      <c r="S31">
-        <v>2.6780705273302301E-3</v>
-      </c>
-      <c r="T31">
-        <v>0.41539997198849898</v>
-      </c>
-      <c r="U31">
-        <v>9.5578463350326093</v>
-      </c>
-      <c r="V31">
-        <v>20.800000000000399</v>
-      </c>
-      <c r="W31">
-        <v>9866666.6666666698</v>
-      </c>
-      <c r="X31">
-        <v>1032310.66087578</v>
-      </c>
-      <c r="Y31">
-        <v>474358.97435896599</v>
-      </c>
-      <c r="Z31">
-        <v>2.07480318315165</v>
-      </c>
-      <c r="AA31">
-        <v>0.95339663461536805</v>
-      </c>
-      <c r="AB31">
-        <v>1.35240717907565</v>
-      </c>
-      <c r="AC31">
-        <v>0.62144711538460495</v>
-      </c>
-      <c r="AD31">
-        <v>0.391159047615945</v>
-      </c>
-      <c r="AE31">
-        <v>0.45951184303040599</v>
-      </c>
-      <c r="AF31">
-        <v>7.5175763326653697E-2</v>
-      </c>
-      <c r="AG31">
-        <v>6.3993301658407595E-2</v>
-      </c>
-      <c r="AH31" s="2">
-        <v>2.0098631756756798E-6</v>
-      </c>
-      <c r="AI31" s="2">
-        <v>1.3100777027027E-6</v>
+      <c r="R34" t="s">
+        <v>66</v>
+      </c>
+      <c r="S34" t="s">
+        <v>67</v>
+      </c>
+      <c r="T34" t="s">
+        <v>16</v>
+      </c>
+      <c r="U34" t="s">
+        <v>17</v>
+      </c>
+      <c r="V34" t="s">
+        <v>18</v>
+      </c>
+      <c r="W34" t="s">
+        <v>19</v>
+      </c>
+      <c r="X34" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI34" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>18</v>
-      </c>
-      <c r="B32" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="1">
-        <v>43831</v>
-      </c>
-      <c r="F32" t="s">
-        <v>35</v>
-      </c>
-      <c r="G32" t="s">
-        <v>36</v>
-      </c>
-      <c r="H32">
-        <v>0.118145705056098</v>
-      </c>
-      <c r="I32">
-        <v>1.62711338153373</v>
-      </c>
-      <c r="J32">
-        <v>1.1796572016118601</v>
-      </c>
-      <c r="K32">
-        <v>390.73500744149101</v>
-      </c>
-      <c r="L32">
-        <v>463.48324672986001</v>
-      </c>
-      <c r="M32">
-        <v>2.0295595375387299</v>
-      </c>
-      <c r="N32">
-        <v>1.7943806371553099</v>
-      </c>
-      <c r="O32">
-        <v>474.27945999201802</v>
-      </c>
-      <c r="P32">
-        <v>15.364633026640099</v>
-      </c>
-      <c r="Q32">
-        <v>698302.82624152605</v>
-      </c>
-      <c r="R32">
-        <v>0.99959557245467501</v>
-      </c>
-      <c r="S32">
-        <v>2.7294530307438599E-3</v>
-      </c>
-      <c r="T32">
-        <v>0.434660122006084</v>
-      </c>
-      <c r="U32">
-        <v>7.2871298548504004</v>
-      </c>
-      <c r="V32">
-        <v>25.000000000001201</v>
-      </c>
-      <c r="W32">
-        <v>10729166.6666667</v>
-      </c>
-      <c r="X32">
-        <v>1472344.65151259</v>
-      </c>
-      <c r="Y32">
-        <v>429166.66666664602</v>
-      </c>
-      <c r="Z32">
-        <v>4.2792482254510604</v>
-      </c>
-      <c r="AA32">
-        <v>1.24733749999994</v>
-      </c>
-      <c r="AB32">
-        <v>3.7833825592732002</v>
-      </c>
-      <c r="AC32">
-        <v>1.10279999999995</v>
-      </c>
-      <c r="AD32">
-        <v>0.47427945999201798</v>
-      </c>
-      <c r="AE32">
-        <v>0.29148519419400098</v>
-      </c>
-      <c r="AF32">
-        <v>3.4437723781464001E-2</v>
-      </c>
-      <c r="AG32">
-        <v>5.6034081194382399E-2</v>
-      </c>
-      <c r="AH32" s="2">
-        <v>2.9064174757281601E-6</v>
-      </c>
-      <c r="AI32" s="2">
-        <v>2.5696310679611601E-6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="35" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" s="4">
+        <v>202.33141289074101</v>
+      </c>
+      <c r="K35" s="4">
+        <v>69.533622499905505</v>
+      </c>
+      <c r="L35" s="4">
+        <v>94534.602067399202</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0.48861573100968603</v>
+      </c>
+      <c r="N35" s="4">
+        <v>1.2512142801114801E-3</v>
+      </c>
+      <c r="O35" s="4">
+        <v>0.114782019524677</v>
+      </c>
+      <c r="P35" s="6">
+        <v>44136</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="T35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="1">
-        <v>43831</v>
-      </c>
-      <c r="F33" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" t="s">
-        <v>48</v>
-      </c>
-      <c r="H33">
-        <v>0.14520803234691501</v>
-      </c>
-      <c r="I33">
-        <v>1.39281593917236</v>
-      </c>
-      <c r="J33">
-        <v>1.3207737354219999</v>
-      </c>
-      <c r="K33">
-        <v>567.98073436729896</v>
-      </c>
-      <c r="L33">
-        <v>685.60163902360796</v>
-      </c>
-      <c r="M33">
-        <v>2.7960579861651298</v>
-      </c>
-      <c r="N33">
-        <v>3.6854390031857398</v>
-      </c>
-      <c r="O33">
-        <v>617.14146519447399</v>
-      </c>
-      <c r="P33">
-        <v>13.325522402500299</v>
-      </c>
-      <c r="Q33">
-        <v>906245.18209692102</v>
-      </c>
-      <c r="R33">
-        <v>1.1238176537978899</v>
-      </c>
-      <c r="S33">
-        <v>3.3335935485625302E-3</v>
-      </c>
-      <c r="T33">
-        <v>0.60752824656641302</v>
-      </c>
-      <c r="U33">
-        <v>8.2237324199608093</v>
-      </c>
-      <c r="V33">
-        <v>18.560000000000802</v>
-      </c>
-      <c r="W33">
-        <v>12076190.4761905</v>
-      </c>
-      <c r="X33">
-        <v>1468456.1534223701</v>
-      </c>
-      <c r="Y33">
-        <v>650656.814449889</v>
-      </c>
-      <c r="Z33">
-        <v>4.5306597333952201</v>
-      </c>
-      <c r="AA33">
-        <v>2.0074856321838199</v>
-      </c>
-      <c r="AB33">
-        <v>5.9717896317732997</v>
-      </c>
-      <c r="AC33">
-        <v>2.6460344827585001</v>
-      </c>
-      <c r="AD33">
-        <v>0.61714146519447399</v>
-      </c>
-      <c r="AE33">
-        <v>0.44308903124786903</v>
-      </c>
-      <c r="AF33">
-        <v>6.4340086382003794E-2</v>
-      </c>
-      <c r="AG33">
-        <v>8.9613897840581505E-2</v>
-      </c>
-      <c r="AH33" s="2">
-        <v>3.0853217665615099E-6</v>
-      </c>
-      <c r="AI33" s="2">
-        <v>4.0667129337539404E-6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>59</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="U35" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="1">
-        <v>43831</v>
-      </c>
-      <c r="F34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" t="s">
-        <v>48</v>
-      </c>
-      <c r="H34">
-        <v>0.17300857271987699</v>
-      </c>
-      <c r="I34">
-        <v>1.3006157314800499</v>
-      </c>
-      <c r="J34">
-        <v>1.22521771806093</v>
-      </c>
-      <c r="K34">
-        <v>226.42023429765501</v>
-      </c>
-      <c r="L34">
-        <v>273.93040750338503</v>
-      </c>
-      <c r="M34">
-        <v>1.9605431270987701</v>
-      </c>
-      <c r="N34">
-        <v>1.79311555513381</v>
-      </c>
-      <c r="O34">
-        <v>554.03399555536805</v>
-      </c>
-      <c r="P34">
-        <v>26.525897822826401</v>
-      </c>
-      <c r="Q34">
-        <v>1016825.9865274701</v>
-      </c>
-      <c r="R34">
-        <v>1.4219122130617301</v>
-      </c>
-      <c r="S34">
-        <v>3.0960478508432199E-3</v>
-      </c>
-      <c r="T34">
-        <v>0.64925132544984798</v>
-      </c>
-      <c r="U34">
-        <v>14.696249156474</v>
-      </c>
-      <c r="V34">
-        <v>34.500000000000398</v>
-      </c>
-      <c r="W34">
-        <v>26972222.222222202</v>
-      </c>
-      <c r="X34">
-        <v>1835313.3466262999</v>
-      </c>
-      <c r="Y34">
-        <v>781803.54267309804</v>
-      </c>
-      <c r="Z34">
-        <v>3.5386693647445</v>
-      </c>
-      <c r="AA34">
-        <v>1.5073961352656799</v>
-      </c>
-      <c r="AB34">
-        <v>3.2364720748523301</v>
-      </c>
-      <c r="AC34">
-        <v>1.3786666666666501</v>
-      </c>
-      <c r="AD34">
-        <v>0.55403399555536803</v>
-      </c>
-      <c r="AE34">
-        <v>0.42597823641952998</v>
-      </c>
-      <c r="AF34">
-        <v>7.3697886692673104E-2</v>
-      </c>
-      <c r="AG34">
-        <v>9.5852630809324796E-2</v>
-      </c>
-      <c r="AH34" s="2">
-        <v>1.9281009268795099E-6</v>
-      </c>
-      <c r="AI34" s="2">
-        <v>1.7634438722966001E-6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>63</v>
-      </c>
-      <c r="B35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="1">
-        <v>43831</v>
-      </c>
-      <c r="F35" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" t="s">
-        <v>57</v>
-      </c>
-      <c r="H35">
-        <v>0.115848259320189</v>
-      </c>
-      <c r="I35">
-        <v>1.1061535598938801</v>
-      </c>
-      <c r="J35">
-        <v>0.91055323527847798</v>
-      </c>
-      <c r="K35">
-        <v>320.19098655660099</v>
-      </c>
-      <c r="L35">
-        <v>389.81795728089702</v>
-      </c>
-      <c r="M35">
-        <v>0.89823378724712399</v>
-      </c>
-      <c r="N35">
-        <v>0.35851516050365601</v>
-      </c>
-      <c r="O35">
-        <v>423.348706063836</v>
-      </c>
-      <c r="P35">
-        <v>29.652302527640501</v>
-      </c>
-      <c r="Q35">
-        <v>826242.75053049403</v>
-      </c>
-      <c r="R35">
-        <v>0.91965399481760002</v>
-      </c>
-      <c r="S35">
-        <v>3.5236420866743999E-3</v>
-      </c>
-      <c r="T35">
-        <v>0.50477847293036304</v>
-      </c>
-      <c r="U35">
-        <v>12.553263906890001</v>
-      </c>
-      <c r="V35">
-        <v>32.799999999999898</v>
-      </c>
-      <c r="W35">
-        <v>24500000</v>
-      </c>
-      <c r="X35">
-        <v>1951683.65627626</v>
-      </c>
-      <c r="Y35">
-        <v>746951.21951219696</v>
-      </c>
-      <c r="Z35">
-        <v>2.1217350481559798</v>
-      </c>
-      <c r="AA35">
-        <v>0.81203353658536703</v>
-      </c>
-      <c r="AB35">
-        <v>0.84685545359762104</v>
-      </c>
-      <c r="AC35">
-        <v>0.32410975609756199</v>
-      </c>
-      <c r="AD35">
-        <v>0.42334870606383601</v>
-      </c>
-      <c r="AE35">
-        <v>0.38272146057591599</v>
-      </c>
-      <c r="AF35">
-        <v>4.4337615012200203E-2</v>
-      </c>
-      <c r="AG35">
-        <v>4.9044210682949702E-2</v>
-      </c>
-      <c r="AH35" s="2">
-        <v>1.0871306122448999E-6</v>
-      </c>
-      <c r="AI35" s="2">
-        <v>4.3391020408163301E-7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>84</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="1">
-        <v>43831</v>
-      </c>
-      <c r="F36" t="s">
-        <v>56</v>
-      </c>
-      <c r="G36" t="s">
-        <v>57</v>
-      </c>
-      <c r="H36">
-        <v>0.106621041740164</v>
-      </c>
-      <c r="I36">
-        <v>0.80795751460282095</v>
-      </c>
-      <c r="J36">
-        <v>0.67910222132567</v>
-      </c>
-      <c r="K36">
-        <v>165.04621781058901</v>
-      </c>
-      <c r="L36">
-        <v>200.24809090371599</v>
-      </c>
-      <c r="M36">
-        <v>0.85117801777082602</v>
-      </c>
-      <c r="N36">
-        <v>0.342988412675377</v>
-      </c>
-      <c r="O36">
-        <v>415.97278121295602</v>
-      </c>
-      <c r="P36">
-        <v>28.7143811161963</v>
-      </c>
-      <c r="Q36">
-        <v>563790.27719171601</v>
-      </c>
-      <c r="R36">
-        <v>0.97246464388892795</v>
-      </c>
-      <c r="S36">
-        <v>1.85183860368685E-3</v>
-      </c>
-      <c r="T36">
-        <v>0.58614835737684901</v>
-      </c>
-      <c r="U36">
-        <v>11.9444009737129</v>
-      </c>
-      <c r="V36">
-        <v>23.200000000000099</v>
-      </c>
-      <c r="W36">
-        <v>16188888.888888899</v>
-      </c>
-      <c r="X36">
-        <v>1355353.76989747</v>
-      </c>
-      <c r="Y36">
-        <v>697796.93486589601</v>
-      </c>
-      <c r="Z36">
-        <v>2.0462348889483399</v>
-      </c>
-      <c r="AA36">
-        <v>1.0534935344827501</v>
-      </c>
-      <c r="AB36">
-        <v>0.82454532643996703</v>
-      </c>
-      <c r="AC36">
-        <v>0.42451293103448001</v>
-      </c>
-      <c r="AD36">
-        <v>0.415972781212956</v>
-      </c>
-      <c r="AE36">
-        <v>0.51484486955658904</v>
-      </c>
-      <c r="AF36">
-        <v>5.48932963267025E-2</v>
-      </c>
-      <c r="AG36">
-        <v>4.4351451268478698E-2</v>
-      </c>
-      <c r="AH36" s="2">
-        <v>1.50974227865477E-6</v>
-      </c>
-      <c r="AI36" s="2">
-        <v>6.0836170212766E-7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>19</v>
-      </c>
-      <c r="B37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="1">
-        <v>44136</v>
-      </c>
-      <c r="F37" t="s">
-        <v>35</v>
-      </c>
-      <c r="G37" t="s">
-        <v>36</v>
-      </c>
-      <c r="H37" t="s">
-        <v>37</v>
-      </c>
-      <c r="I37">
-        <v>0.50530402714327105</v>
-      </c>
-      <c r="J37">
-        <v>0.503330183287229</v>
-      </c>
-      <c r="K37">
-        <v>94.570806830031103</v>
-      </c>
-      <c r="L37">
-        <v>113.80196751931599</v>
-      </c>
-      <c r="M37">
-        <v>0.56168095535914497</v>
-      </c>
-      <c r="N37">
-        <v>0.299250519324749</v>
-      </c>
-      <c r="O37" t="s">
-        <v>37</v>
-      </c>
-      <c r="P37">
-        <v>30.3975412324295</v>
-      </c>
-      <c r="Q37">
-        <v>214820.006331087</v>
-      </c>
-      <c r="R37">
-        <v>0.81568123579018903</v>
-      </c>
-      <c r="S37">
-        <v>2.4365068649643798E-3</v>
-      </c>
-      <c r="T37">
-        <v>0.34856854250958602</v>
-      </c>
-      <c r="U37" t="s">
-        <v>37</v>
-      </c>
-      <c r="V37">
-        <v>15.3600000000003</v>
-      </c>
-      <c r="W37">
-        <v>6530000</v>
-      </c>
-      <c r="X37" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y37">
-        <v>425130.20833332598</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA37">
-        <v>1.1115703124999801</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC37">
-        <v>0.59221874999999102</v>
-      </c>
-      <c r="AD37" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE37" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF37" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG37" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH37" s="2">
-        <v>2.6146584992343101E-6</v>
-      </c>
-      <c r="AI37" s="2">
-        <v>1.3930290964778E-6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>60</v>
-      </c>
-      <c r="B38" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="1">
-        <v>44136</v>
-      </c>
-      <c r="F38" t="s">
-        <v>47</v>
-      </c>
-      <c r="G38" t="s">
-        <v>48</v>
-      </c>
-      <c r="H38" t="s">
-        <v>37</v>
-      </c>
-      <c r="I38">
-        <v>1.2957911441005101</v>
-      </c>
-      <c r="J38">
-        <v>0.54482127649676604</v>
-      </c>
-      <c r="K38">
-        <v>93.391201731172899</v>
-      </c>
-      <c r="L38">
-        <v>169.05656960702501</v>
-      </c>
-      <c r="M38">
-        <v>0.640397653293721</v>
-      </c>
-      <c r="N38">
-        <v>0.32713130926779799</v>
-      </c>
-      <c r="O38">
-        <v>346.68071258500601</v>
-      </c>
-      <c r="P38">
-        <v>63.667667722229297</v>
-      </c>
-      <c r="Q38">
-        <v>196086.576540971</v>
-      </c>
-      <c r="R38">
-        <v>0.44145099385251901</v>
-      </c>
-      <c r="S38">
-        <v>1.0675887644996599E-3</v>
-      </c>
-      <c r="T38">
-        <v>0.18757983587997401</v>
-      </c>
-      <c r="U38">
-        <v>22.072352414567799</v>
-      </c>
-      <c r="V38">
-        <v>82.499999999998707</v>
-      </c>
-      <c r="W38">
-        <v>12484375</v>
-      </c>
-      <c r="X38">
-        <v>565611.43848719401</v>
-      </c>
-      <c r="Y38">
-        <v>151325.75757576001</v>
-      </c>
-      <c r="Z38">
-        <v>1.84722607877038</v>
-      </c>
-      <c r="AA38">
-        <v>0.49421363636364402</v>
-      </c>
-      <c r="AB38">
-        <v>0.94360977519793698</v>
-      </c>
-      <c r="AC38">
-        <v>0.25245681818182197</v>
-      </c>
-      <c r="AD38">
-        <v>0.34668071258500599</v>
-      </c>
-      <c r="AE38">
-        <v>0.26754366563112902</v>
-      </c>
-      <c r="AF38" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG38" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH38" s="2">
-        <v>3.2658923654568202E-6</v>
-      </c>
-      <c r="AI38" s="2">
-        <v>1.6683003754693401E-6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="1">
-        <v>44136</v>
-      </c>
-      <c r="F39" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39">
-        <v>0.19146997167881399</v>
-      </c>
-      <c r="I39">
-        <v>0.693497776956703</v>
-      </c>
-      <c r="J39">
-        <v>0.735195428102834</v>
-      </c>
-      <c r="K39">
-        <v>103.87543284466599</v>
-      </c>
-      <c r="L39">
-        <v>126.22317924577401</v>
-      </c>
-      <c r="M39">
-        <v>0.67091959616768004</v>
-      </c>
-      <c r="N39">
-        <v>0.26487445314631403</v>
-      </c>
-      <c r="O39">
-        <v>253.40421317115599</v>
-      </c>
-      <c r="P39">
-        <v>45.566115782910401</v>
-      </c>
-      <c r="Q39">
-        <v>196539.80598702599</v>
-      </c>
-      <c r="R39">
-        <v>0.73990593858654796</v>
-      </c>
-      <c r="S39">
-        <v>2.3155231556607602E-3</v>
-      </c>
-      <c r="T39">
-        <v>0.232428594429613</v>
-      </c>
-      <c r="U39">
-        <v>11.546645717234201</v>
-      </c>
-      <c r="V39">
-        <v>31.600000000000101</v>
-      </c>
-      <c r="W39">
-        <v>8955555.5555555597</v>
-      </c>
-      <c r="X39">
-        <v>775598.01996771595</v>
-      </c>
-      <c r="Y39">
-        <v>283403.65682137798</v>
-      </c>
-      <c r="Z39">
-        <v>2.64762605077336</v>
-      </c>
-      <c r="AA39">
-        <v>0.96744303797468101</v>
-      </c>
-      <c r="AB39">
-        <v>1.0452645985306099</v>
-      </c>
-      <c r="AC39">
-        <v>0.38193987341772001</v>
-      </c>
-      <c r="AD39">
-        <v>0.25340421317115602</v>
-      </c>
-      <c r="AE39">
-        <v>0.36540018092513199</v>
-      </c>
-      <c r="AF39">
-        <v>6.9963162293168402E-2</v>
-      </c>
-      <c r="AG39">
-        <v>4.8519297519173298E-2</v>
-      </c>
-      <c r="AH39" s="2">
-        <v>3.4136575682382101E-6</v>
-      </c>
-      <c r="AI39" s="2">
-        <v>1.3476885856079399E-6</v>
+      <c r="V35" s="4">
+        <v>14.068836083817301</v>
+      </c>
+      <c r="W35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="X35" s="4">
+        <v>6573333.3333333302</v>
+      </c>
+      <c r="Y35" s="4">
+        <v>467226.520671051</v>
+      </c>
+      <c r="Z35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE35" s="4">
+        <v>0.202331412890741</v>
+      </c>
+      <c r="AF35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI35" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ35" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI41">
-    <sortCondition ref="C2:C41"/>
-    <sortCondition ref="D2:D41"/>
-    <sortCondition ref="F2:F41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI33">
+    <sortCondition ref="C2:C33"/>
+    <sortCondition ref="D2:D33"/>
+    <sortCondition ref="F2:F33"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>